<commit_message>
Mudanças a serem submetidas:
</commit_message>
<xml_diff>
--- a/dados_extraidos.xlsx
+++ b/dados_extraidos.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Base de dados"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="73">
   <si>
     <t>Pagina</t>
   </si>
@@ -166,19 +166,19 @@
     <t>Page 0</t>
   </si>
   <si>
-    <t>2000101612, 0044108909</t>
-  </si>
-  <si>
-    <t>JARDIM , 15698, DO ESPIRITO SANTO , S/N</t>
+    <t>0044108909, 2000101612</t>
+  </si>
+  <si>
+    <t>DO ESPIRITO SANTO , S/N, JARDIM , 15698</t>
   </si>
   <si>
     <t>SAO MIGUEL, VILA ESPERANCA</t>
   </si>
   <si>
-    <t>SAAE CAXIAS, POCO ARTESIANO VILA ESPERANCA CAXIAS</t>
-  </si>
-  <si>
-    <t>0202409096594631, 0202409096486293</t>
+    <t>POCO ARTESIANO VILA ESPERANCA CAXIAS, SAAE CAXIAS</t>
+  </si>
+  <si>
+    <t>0202409096486293, 0202409096594631</t>
   </si>
   <si>
     <t>05, 07</t>
@@ -187,13 +187,13 @@
     <t>5038411600, 7013600601</t>
   </si>
   <si>
-    <t>B3, B3</t>
+    <t>B3</t>
   </si>
   <si>
     <t>1,00, 3,00</t>
   </si>
   <si>
-    <t>26/09/2024, 25/09/2024</t>
+    <t>25/09/2024, 26/09/2024</t>
   </si>
   <si>
     <t>30, 32</t>
@@ -205,25 +205,28 @@
     <t>20/09/2024</t>
   </si>
   <si>
-    <t>29.44, 0.00</t>
-  </si>
-  <si>
-    <t>22.96, 0.00</t>
-  </si>
-  <si>
-    <t>Medidor, Medidor</t>
-  </si>
-  <si>
-    <t>Cte., Cte.</t>
+    <t>('0.00', '22,0000', '0.00'), ('29.44', '22,0000', '6.48')</t>
+  </si>
+  <si>
+    <t>('0.00', '2,5363', '0.00'), ('22.96', '2,5363', '0.58')</t>
+  </si>
+  <si>
+    <t>('0.00', '0,5489', '0.00'), ('22.96', '0,5489', '0.13')</t>
+  </si>
+  <si>
+    <t>Medidor</t>
+  </si>
+  <si>
+    <t>Cte.</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Leit., Leit.</t>
-  </si>
-  <si>
-    <t>Faturado, Faturado</t>
+    <t>Leit.</t>
+  </si>
+  <si>
+    <t>Faturado</t>
   </si>
   <si>
     <t>30,00</t>
@@ -235,10 +238,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -254,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -262,29 +272,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -293,10 +310,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -334,71 +351,69 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,53 +437,54 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="51000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
+                <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="94000"/>
+                <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="9500"/>
+              <a:shade val="95000"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -478,7 +494,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -487,7 +503,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -496,7 +512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -504,10 +520,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -536,7 +552,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="20000"/>
+                <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -549,12 +565,13 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -572,68 +589,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="26.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="2" width="11.862142857142858" customWidth="1" bestFit="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="16.5">
+    <row r="1" spans="1:49">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,153 +745,153 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:49">
+      <c r="A2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>61</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" t="s">
         <v>63</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" t="s">
         <v>63</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" t="s">
         <v>64</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="U2" t="s">
         <v>65</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="V2" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" t="s">
         <v>66</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Y2" t="s">
         <v>67</v>
       </c>
-      <c r="AA2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD2" s="1" t="s">
+      <c r="Z2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA2" t="s">
         <v>69</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AB2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" t="s">
         <v>70</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AE2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" t="s">
         <v>71</v>
       </c>
-      <c r="AJ2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>67</v>
+      <c r="AG2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Erro de busca de data como erro de ortografico(Dta\Dat) corrigido
</commit_message>
<xml_diff>
--- a/dados_extraidos.xlsx
+++ b/dados_extraidos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="443">
   <si>
     <t>Página-Arquivo</t>
   </si>
@@ -1306,12 +1306,18 @@
     <t>21/08/2024</t>
   </si>
   <si>
+    <t>23/08/2024</t>
+  </si>
+  <si>
     <t>16/08/2024</t>
   </si>
   <si>
     <t>29/08/2024</t>
   </si>
   <si>
+    <t>02/08/2024</t>
+  </si>
+  <si>
     <t>26/08/2024</t>
   </si>
   <si>
@@ -1324,25 +1330,19 @@
     <t>13/08/2024</t>
   </si>
   <si>
+    <t>14/08/2024</t>
+  </si>
+  <si>
     <t>09/08/2024</t>
   </si>
   <si>
+    <t>19/08/2024</t>
+  </si>
+  <si>
     <t>22/08/2024</t>
   </si>
   <si>
-    <t>19/08/2024</t>
-  </si>
-  <si>
-    <t>02/08/2024</t>
-  </si>
-  <si>
-    <t>14/08/2024</t>
-  </si>
-  <si>
     <t>15/08/2024</t>
-  </si>
-  <si>
-    <t>23/08/2024</t>
   </si>
 </sst>
 </file>
@@ -1831,6 +1831,12 @@
       <c r="L3" t="s">
         <v>424</v>
       </c>
+      <c r="M3" t="s">
+        <v>430</v>
+      </c>
+      <c r="N3" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
@@ -1870,7 +1876,7 @@
         <v>424</v>
       </c>
       <c r="M4" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N4" t="s">
         <v>405</v>
@@ -1913,6 +1919,12 @@
       <c r="L5" t="s">
         <v>424</v>
       </c>
+      <c r="M5" t="s">
+        <v>431</v>
+      </c>
+      <c r="N5" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
@@ -1952,7 +1964,7 @@
         <v>425</v>
       </c>
       <c r="M6" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="N6" t="s">
         <v>422</v>
@@ -1995,6 +2007,12 @@
       <c r="L7" t="s">
         <v>424</v>
       </c>
+      <c r="M7" t="s">
+        <v>433</v>
+      </c>
+      <c r="N7" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
@@ -2034,7 +2052,7 @@
         <v>426</v>
       </c>
       <c r="M8" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="N8" t="s">
         <v>403</v>
@@ -2077,6 +2095,12 @@
       <c r="L9" t="s">
         <v>426</v>
       </c>
+      <c r="M9" t="s">
+        <v>434</v>
+      </c>
+      <c r="N9" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
@@ -2116,7 +2140,7 @@
         <v>426</v>
       </c>
       <c r="M10" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="N10" t="s">
         <v>408</v>
@@ -2159,6 +2183,12 @@
       <c r="L11" t="s">
         <v>424</v>
       </c>
+      <c r="M11" t="s">
+        <v>430</v>
+      </c>
+      <c r="N11" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
@@ -2241,6 +2271,12 @@
       <c r="L13" t="s">
         <v>423</v>
       </c>
+      <c r="M13" t="s">
+        <v>429</v>
+      </c>
+      <c r="N13" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
@@ -2280,7 +2316,7 @@
         <v>427</v>
       </c>
       <c r="M14" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="N14" t="s">
         <v>410</v>
@@ -2323,6 +2359,12 @@
       <c r="L15" t="s">
         <v>427</v>
       </c>
+      <c r="M15" t="s">
+        <v>436</v>
+      </c>
+      <c r="N15" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
@@ -2362,7 +2404,7 @@
         <v>426</v>
       </c>
       <c r="M16" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="N16" t="s">
         <v>421</v>
@@ -2405,6 +2447,12 @@
       <c r="L17" t="s">
         <v>426</v>
       </c>
+      <c r="M17" t="s">
+        <v>438</v>
+      </c>
+      <c r="N17" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
@@ -2444,7 +2492,7 @@
         <v>426</v>
       </c>
       <c r="M18" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="N18" t="s">
         <v>408</v>
@@ -2487,6 +2535,12 @@
       <c r="L19" t="s">
         <v>424</v>
       </c>
+      <c r="M19" t="s">
+        <v>433</v>
+      </c>
+      <c r="N19" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
@@ -2526,7 +2580,7 @@
         <v>427</v>
       </c>
       <c r="M20" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="N20" t="s">
         <v>416</v>
@@ -2569,6 +2623,12 @@
       <c r="L21" t="s">
         <v>426</v>
       </c>
+      <c r="M21" t="s">
+        <v>437</v>
+      </c>
+      <c r="N21" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
@@ -2608,7 +2668,7 @@
         <v>426</v>
       </c>
       <c r="M22" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="N22" t="s">
         <v>421</v>
@@ -2651,6 +2711,12 @@
       <c r="L23" t="s">
         <v>424</v>
       </c>
+      <c r="M23" t="s">
+        <v>431</v>
+      </c>
+      <c r="N23" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="24" spans="1:14">
       <c r="A24" t="s">
@@ -2690,7 +2756,7 @@
         <v>424</v>
       </c>
       <c r="M24" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N24" t="s">
         <v>405</v>
@@ -2733,6 +2799,12 @@
       <c r="L25" t="s">
         <v>427</v>
       </c>
+      <c r="M25" t="s">
+        <v>436</v>
+      </c>
+      <c r="N25" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="26" spans="1:14">
       <c r="A26" t="s">
@@ -2772,7 +2844,7 @@
         <v>427</v>
       </c>
       <c r="M26" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="N26" t="s">
         <v>416</v>
@@ -2815,6 +2887,12 @@
       <c r="L27" t="s">
         <v>427</v>
       </c>
+      <c r="M27" t="s">
+        <v>436</v>
+      </c>
+      <c r="N27" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
@@ -2854,7 +2932,7 @@
         <v>427</v>
       </c>
       <c r="M28" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="N28" t="s">
         <v>410</v>
@@ -2897,6 +2975,12 @@
       <c r="L29" t="s">
         <v>423</v>
       </c>
+      <c r="M29" t="s">
+        <v>429</v>
+      </c>
+      <c r="N29" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
@@ -2936,7 +3020,7 @@
         <v>424</v>
       </c>
       <c r="M30" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N30" t="s">
         <v>405</v>
@@ -2979,6 +3063,12 @@
       <c r="L31" t="s">
         <v>423</v>
       </c>
+      <c r="M31" t="s">
+        <v>440</v>
+      </c>
+      <c r="N31" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
@@ -3018,7 +3108,7 @@
         <v>424</v>
       </c>
       <c r="M32" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N32" t="s">
         <v>405</v>
@@ -3061,6 +3151,12 @@
       <c r="L33" t="s">
         <v>423</v>
       </c>
+      <c r="M33" t="s">
+        <v>440</v>
+      </c>
+      <c r="N33" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
@@ -3100,7 +3196,7 @@
         <v>426</v>
       </c>
       <c r="M34" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="N34" t="s">
         <v>403</v>
@@ -3143,6 +3239,12 @@
       <c r="L35" t="s">
         <v>423</v>
       </c>
+      <c r="M35" t="s">
+        <v>429</v>
+      </c>
+      <c r="N35" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
@@ -3182,7 +3284,7 @@
         <v>424</v>
       </c>
       <c r="M36" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="N36" t="s">
         <v>419</v>
@@ -3225,6 +3327,12 @@
       <c r="L37" t="s">
         <v>423</v>
       </c>
+      <c r="M37" t="s">
+        <v>440</v>
+      </c>
+      <c r="N37" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
@@ -3264,7 +3372,7 @@
         <v>423</v>
       </c>
       <c r="M38" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N38" t="s">
         <v>417</v>
@@ -3307,6 +3415,12 @@
       <c r="L39" t="s">
         <v>423</v>
       </c>
+      <c r="M39" t="s">
+        <v>440</v>
+      </c>
+      <c r="N39" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
@@ -3346,7 +3460,7 @@
         <v>424</v>
       </c>
       <c r="M40" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="N40" t="s">
         <v>412</v>
@@ -3389,6 +3503,12 @@
       <c r="L41" t="s">
         <v>424</v>
       </c>
+      <c r="M41" t="s">
+        <v>433</v>
+      </c>
+      <c r="N41" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
@@ -3428,7 +3548,7 @@
         <v>424</v>
       </c>
       <c r="M42" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="N42" t="s">
         <v>412</v>
@@ -3471,6 +3591,12 @@
       <c r="L43" t="s">
         <v>423</v>
       </c>
+      <c r="M43" t="s">
+        <v>440</v>
+      </c>
+      <c r="N43" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
@@ -3510,7 +3636,7 @@
         <v>427</v>
       </c>
       <c r="M44" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="N44" t="s">
         <v>410</v>
@@ -3553,6 +3679,12 @@
       <c r="L45" t="s">
         <v>427</v>
       </c>
+      <c r="M45" t="s">
+        <v>436</v>
+      </c>
+      <c r="N45" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
@@ -3592,7 +3724,7 @@
         <v>427</v>
       </c>
       <c r="M46" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="N46" t="s">
         <v>416</v>
@@ -3635,6 +3767,12 @@
       <c r="L47" t="s">
         <v>427</v>
       </c>
+      <c r="M47" t="s">
+        <v>439</v>
+      </c>
+      <c r="N47" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
@@ -3674,7 +3812,7 @@
         <v>427</v>
       </c>
       <c r="M48" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="N48" t="s">
         <v>410</v>
@@ -3717,6 +3855,12 @@
       <c r="L49" t="s">
         <v>427</v>
       </c>
+      <c r="M49" t="s">
+        <v>436</v>
+      </c>
+      <c r="N49" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
@@ -3756,7 +3900,7 @@
         <v>427</v>
       </c>
       <c r="M50" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="N50" t="s">
         <v>410</v>
@@ -3799,6 +3943,12 @@
       <c r="L51" t="s">
         <v>427</v>
       </c>
+      <c r="M51" t="s">
+        <v>436</v>
+      </c>
+      <c r="N51" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
@@ -3838,7 +3988,7 @@
         <v>426</v>
       </c>
       <c r="M52" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="N52" t="s">
         <v>421</v>
@@ -3881,6 +4031,12 @@
       <c r="L53" t="s">
         <v>426</v>
       </c>
+      <c r="M53" t="s">
+        <v>437</v>
+      </c>
+      <c r="N53" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
@@ -3920,7 +4076,7 @@
         <v>426</v>
       </c>
       <c r="M54" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="N54" t="s">
         <v>411</v>
@@ -3963,6 +4119,12 @@
       <c r="L55" t="s">
         <v>426</v>
       </c>
+      <c r="M55" t="s">
+        <v>438</v>
+      </c>
+      <c r="N55" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
@@ -4002,7 +4164,7 @@
         <v>426</v>
       </c>
       <c r="M56" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="N56" t="s">
         <v>411</v>
@@ -4045,6 +4207,12 @@
       <c r="L57" t="s">
         <v>426</v>
       </c>
+      <c r="M57" t="s">
+        <v>438</v>
+      </c>
+      <c r="N57" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="58" spans="1:14">
       <c r="A58" t="s">
@@ -4084,7 +4252,7 @@
         <v>426</v>
       </c>
       <c r="M58" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="N58" t="s">
         <v>411</v>
@@ -4127,6 +4295,12 @@
       <c r="L59" t="s">
         <v>426</v>
       </c>
+      <c r="M59" t="s">
+        <v>438</v>
+      </c>
+      <c r="N59" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="60" spans="1:14">
       <c r="A60" t="s">
@@ -4166,7 +4340,7 @@
         <v>426</v>
       </c>
       <c r="M60" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="N60" t="s">
         <v>421</v>
@@ -4209,6 +4383,12 @@
       <c r="L61" t="s">
         <v>426</v>
       </c>
+      <c r="M61" t="s">
+        <v>438</v>
+      </c>
+      <c r="N61" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="62" spans="1:14">
       <c r="A62" t="s">
@@ -4248,7 +4428,7 @@
         <v>424</v>
       </c>
       <c r="M62" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="N62" t="s">
         <v>414</v>
@@ -4291,6 +4471,12 @@
       <c r="L63" t="s">
         <v>426</v>
       </c>
+      <c r="M63" t="s">
+        <v>437</v>
+      </c>
+      <c r="N63" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="64" spans="1:14">
       <c r="A64" t="s">
@@ -4330,7 +4516,7 @@
         <v>426</v>
       </c>
       <c r="M64" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="N64" t="s">
         <v>421</v>
@@ -4373,6 +4559,12 @@
       <c r="L65" t="s">
         <v>424</v>
       </c>
+      <c r="M65" t="s">
+        <v>431</v>
+      </c>
+      <c r="N65" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="66" spans="1:14">
       <c r="A66" t="s">
@@ -4412,7 +4604,7 @@
         <v>424</v>
       </c>
       <c r="M66" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="N66" t="s">
         <v>405</v>
@@ -4455,6 +4647,12 @@
       <c r="L67" t="s">
         <v>426</v>
       </c>
+      <c r="M67" t="s">
+        <v>437</v>
+      </c>
+      <c r="N67" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="68" spans="1:14">
       <c r="A68" t="s">
@@ -4494,7 +4692,7 @@
         <v>423</v>
       </c>
       <c r="M68" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N68" t="s">
         <v>417</v>
@@ -4537,6 +4735,12 @@
       <c r="L69" t="s">
         <v>423</v>
       </c>
+      <c r="M69" t="s">
+        <v>440</v>
+      </c>
+      <c r="N69" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="70" spans="1:14">
       <c r="A70" t="s">
@@ -4576,7 +4780,7 @@
         <v>423</v>
       </c>
       <c r="M70" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N70" t="s">
         <v>417</v>
@@ -4619,6 +4823,12 @@
       <c r="L71" t="s">
         <v>423</v>
       </c>
+      <c r="M71" t="s">
+        <v>440</v>
+      </c>
+      <c r="N71" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="72" spans="1:14">
       <c r="A72" t="s">
@@ -4658,7 +4868,7 @@
         <v>424</v>
       </c>
       <c r="M72" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="N72" t="s">
         <v>409</v>
@@ -4701,6 +4911,12 @@
       <c r="L73" t="s">
         <v>423</v>
       </c>
+      <c r="M73" t="s">
+        <v>429</v>
+      </c>
+      <c r="N73" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="74" spans="1:14">
       <c r="A74" t="s">
@@ -4740,7 +4956,7 @@
         <v>424</v>
       </c>
       <c r="M74" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="N74" t="s">
         <v>409</v>
@@ -4783,6 +4999,12 @@
       <c r="L75" t="s">
         <v>424</v>
       </c>
+      <c r="M75" t="s">
+        <v>430</v>
+      </c>
+      <c r="N75" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" t="s">
@@ -4822,7 +5044,7 @@
         <v>424</v>
       </c>
       <c r="M76" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="N76" t="s">
         <v>409</v>
@@ -4862,6 +5084,12 @@
       <c r="L77" t="s">
         <v>424</v>
       </c>
+      <c r="M77" t="s">
+        <v>430</v>
+      </c>
+      <c r="N77" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="78" spans="1:14">
       <c r="A78" t="s">
@@ -4901,7 +5129,7 @@
         <v>426</v>
       </c>
       <c r="M78" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="N78" t="s">
         <v>403</v>
@@ -4944,6 +5172,12 @@
       <c r="L79" t="s">
         <v>428</v>
       </c>
+      <c r="M79" t="s">
+        <v>440</v>
+      </c>
+      <c r="N79" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="80" spans="1:14">
       <c r="A80" t="s">
@@ -4983,13 +5217,13 @@
         <v>425</v>
       </c>
       <c r="M80" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="N80" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:14">
       <c r="A81" t="s">
         <v>53</v>
       </c>
@@ -5025,6 +5259,12 @@
       </c>
       <c r="L81" t="s">
         <v>426</v>
+      </c>
+      <c r="M81" t="s">
+        <v>434</v>
+      </c>
+      <c r="N81" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>